<commit_message>
Modified dummy controls so that the difference between cyclo and noncyclo is more easily captured by PCA
</commit_message>
<xml_diff>
--- a/Cyclo_noncyclo_comparison/Examples/example2/Inputs/create_read_stat/madeup_positive_controls.xlsx
+++ b/Cyclo_noncyclo_comparison/Examples/example2/Inputs/create_read_stat/madeup_positive_controls.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hank\Documents\Research\Projects\Iso-seq_public\Cyclo_noncyclo_comparison\Examples\Example2\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hank\AppData\Local\Temp\scp31772\mmfs1\gscratch\stergachislab\yhhc\projects\Iso-seq_public\Cyclo_noncyclo_comparison\Examples\example2\Inputs\create_read_stat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7536AE-70E2-4075-B8C2-726B816265A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3440336B-13E5-4A4C-9A65-3C7CA2D4B48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B63E0232-D77F-4A71-81C7-BBF627DB2C1D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{B63E0232-D77F-4A71-81C7-BBF627DB2C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
   <si>
     <t>Hyp1</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>GeneF</t>
+  </si>
+  <si>
+    <t>PB.19</t>
+  </si>
+  <si>
+    <t>GeneJ</t>
   </si>
 </sst>
 </file>
@@ -314,12 +320,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFCBB26-0AD6-4E71-9ACB-E85936D88997}">
-  <dimension ref="A2:K34"/>
+  <dimension ref="A2:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,38 +741,38 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -777,73 +781,73 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -852,73 +856,73 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" t="s">
         <v>58</v>
       </c>
     </row>
@@ -927,38 +931,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1088,6 +1092,14 @@
       </c>
       <c r="B34" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1098,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486AF542-DBFA-4B1A-8BC6-E9C5CB8E5113}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1625,6 +1637,35 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>2000</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2000</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2000</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2000</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>